<commit_message>
Created table with texture classification.
</commit_message>
<xml_diff>
--- a/01_input/soil_data_combined_2025_02_04.xlsx
+++ b/01_input/soil_data_combined_2025_02_04.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
   <si>
     <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hplus_conc_mol_l</t>
   </si>
   <si>
     <t xml:space="preserve">clay</t>
@@ -608,2748 +611,2847 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
         <v>4.86</v>
       </c>
       <c r="C2" t="n">
+        <v>0.0000138038426460288</v>
+      </c>
+      <c r="D2" t="n">
         <v>7.95733333333333</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>47.102</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>44.9403333333333</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>341.800228908563</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>47.4510462493498</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>1415.43509861132</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>70.6340185943071</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.236814535716836</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>2.12990993423722</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>3.14427535008173</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>122.934877637496</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>11.5174936818572</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>139.966341968769</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>1.62565086974287</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>44.655003740967</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.577069104384793</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>13.2668187098064</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>86.1096712663476</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.19</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>1.56666666666667</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>8.33736666666667</v>
       </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2"/>
-      <c r="Z2" t="n">
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2"/>
+      <c r="AA2" t="n">
         <v>1.56666666666667</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>2.69466666666667</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>1.22391929333082</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="n">
         <v>6.12</v>
       </c>
       <c r="C3" t="n">
+        <v>0.000000758577575029184</v>
+      </c>
+      <c r="D3" t="n">
         <v>13.1145</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>58.704</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>28.182</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>437.511272344968</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>98.8572808527078</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>2700.39076307767</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>134.756762467073</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.0147414075105099</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.132584219149526</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>7.52754650714104</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>294.3120133362</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>19.1846747166728</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>233.141759494366</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.950770915085221</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>26.1167262664759</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.879803131131759</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>20.2266739847191</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>162.363528229529</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.3</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>2.705</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>8.90625</v>
       </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
       <c r="Y3" t="n">
         <v>0</v>
       </c>
       <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
         <v>2.705</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>4.6526</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>1.15094660843231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="n">
         <v>7.28</v>
       </c>
       <c r="C4" t="n">
+        <v>0.0000000524807460249772</v>
+      </c>
+      <c r="D4" t="n">
         <v>7.695</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>38.739</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>53.566</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>322.567065776777</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>66.6604361365048</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>4618.78131166493</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>230.489610842104</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.0438445770388414</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.39433812588734</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>3.4174887695597</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>133.616975912245</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>4.86473232822269</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>59.1186596187263</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>0.163293412060965</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>4.48550673590264</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>0.4223280716346</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>9.70932236687946</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>239.23800458856</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>0.16</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>1.845</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>11.63805</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>0.39</v>
       </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
       <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
         <v>1.455</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>2.5026</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>1.41165682494325</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>5.06</v>
       </c>
       <c r="C5" t="n">
+        <v>0.00000870963589956081</v>
+      </c>
+      <c r="D5" t="n">
         <v>9.6745</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>41.8885</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>48.437</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>310.203278474351</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>84.4735397052181</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>1217.04486715729</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>60.7338124236386</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>1.00007494852091</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>8.99467408699704</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>3.12618322297882</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>122.227511652026</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>7.1588497740689</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>86.9979218793724</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>0.473772036042461</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>13.0140440580504</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>0.368192952160386</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>8.46475597016727</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>72.3871133213677</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>0.26</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>2.62</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>9.96285</v>
       </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
       <c r="Y5" t="n">
         <v>0</v>
       </c>
       <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
         <v>2.62</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>4.5064</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>1.05425348194723</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="n">
         <v>6.69</v>
       </c>
       <c r="C6" t="n">
+        <v>0.000000204173794466953</v>
+      </c>
+      <c r="D6" t="n">
         <v>13.9546666666667</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>72.4033333333333</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>13.642</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>383.108726720474</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>86.1586079244115</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>4056.58738640374</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>202.434621807662</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.0110908294682419</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.0997509202373677</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>11.1351233487296</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>435.361052688631</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>15.3812100567169</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>186.920155214252</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.160896093076851</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>4.41965478072801</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>0.575850331120971</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>13.2387991124711</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>229.537896373698</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>0.31</v>
       </c>
-      <c r="V6" t="n">
+      <c r="W6" t="n">
         <v>3.025</v>
       </c>
-      <c r="W6" t="n">
+      <c r="X6" t="n">
         <v>9.67215</v>
       </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
       <c r="Y6" t="n">
         <v>0</v>
       </c>
       <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
         <v>3.025</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>5.203</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>1.12037336215874</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="n">
         <v>5.09</v>
       </c>
       <c r="C7" t="n">
+        <v>0.00000812830516164099</v>
+      </c>
+      <c r="D7" t="n">
         <v>8.13233333333333</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>62.693</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>29.1746666666667</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>228.706593082627</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>35.1130009148313</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>1465.24222550307</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>73.1195281951727</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.100890328474627</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.907407614300795</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>7.73697672313286</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>302.500315921049</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>12.3858696952682</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>150.519281471747</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>1.30933169500251</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>35.966032330024</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>0.466254671655897</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>10.7191949013691</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>93.8095196137043</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>0.176666666666667</v>
       </c>
-      <c r="V7" t="n">
+      <c r="W7" t="n">
         <v>1.64666666666667</v>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>9.2569</v>
       </c>
-      <c r="X7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7"/>
-      <c r="Z7" t="n">
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7"/>
+      <c r="AA7" t="n">
         <v>1.64666666666667</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>2.83226666666667</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>1.37323086130489</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="n">
         <v>5.42</v>
       </c>
       <c r="C8" t="n">
+        <v>0.00000380189396320561</v>
+      </c>
+      <c r="D8" t="n">
         <v>9.95833333333333</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>64.3736666666667</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>25.6683333333333</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>290.733422410904</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>61.4292829874568</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>2060.58960359094</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>102.828963700331</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.121893446668865</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>1.09630965933977</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>8.81719546126697</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>344.734708144616</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>21.3868667263891</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>259.903897892444</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>0.498469064006996</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>13.6924467192082</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>0.646610637436099</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>14.8655785546559</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>133.801529972093</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>0.26</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>2.46</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>9.40935</v>
       </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
       <c r="Y8" t="n">
         <v>0</v>
       </c>
       <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
         <v>2.46</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AB8" t="n">
         <v>4.2312</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AC8" t="n">
         <v>1.23601771321751</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="n">
         <v>5.02</v>
       </c>
       <c r="C9" t="n">
+        <v>0.00000954992586021437</v>
+      </c>
+      <c r="D9" t="n">
         <v>11.46</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>63.67</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>24.87</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>267.178844089758</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>50.7320859616461</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>1558.27146266342</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>77.7619373553279</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.310978006056552</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>2.79693618647263</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>3.6579710284449</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>143.019351270139</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>15.8301987345679</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>192.376490121836</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>0.91251578727342</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>25.0658961606136</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>0.420337961237868</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>9.66356972885859</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>97.9814230856351</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>0.24</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>2.195</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>9.12455</v>
       </c>
-      <c r="X9" t="n">
-        <v>0</v>
-      </c>
       <c r="Y9" t="n">
         <v>0</v>
       </c>
       <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
         <v>2.195</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AB9" t="n">
         <v>3.7754</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>1.24303280739672</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="n">
         <v>5.72</v>
       </c>
       <c r="C10" t="n">
+        <v>0.00000190546071796325</v>
+      </c>
+      <c r="D10" t="n">
         <v>12.6016666666667</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>70.3366666666667</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>17.0616666666667</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>371.488887104</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>77.4315224213334</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>2325.42836690833</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>116.045130341251</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.499863085663892</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>4.49576859246105</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>14.213772055122</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>555.730059811158</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>24.2720235999519</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>294.965766798415</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.441624290876033</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>12.1309776460737</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>0.539042402435592</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>12.3925848319943</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>155.569831484424</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>0.29</v>
       </c>
-      <c r="V10" t="n">
+      <c r="W10" t="n">
         <v>2.74</v>
       </c>
-      <c r="W10" t="n">
+      <c r="X10" t="n">
         <v>9.35485</v>
       </c>
-      <c r="X10" t="n">
-        <v>0</v>
-      </c>
       <c r="Y10" t="n">
         <v>0</v>
       </c>
       <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
         <v>2.74</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AB10" t="n">
         <v>4.7128</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AC10" t="n">
         <v>1.19361303944765</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="n">
         <v>5.55</v>
       </c>
       <c r="C11" t="n">
+        <v>0.00000281838293126446</v>
+      </c>
+      <c r="D11" t="n">
         <v>9.5565</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>53.2315</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>37.2115</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>413.64567496964</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>110.70759061149</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>1944.73770248629</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>97.0476422219815</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>1.11261791581027</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>10.0068855347976</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>5.52496736646237</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>216.015174093946</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>13.6064537558744</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>165.352429268264</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>0.683352076162265</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>18.7709981801013</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>0.515446994466642</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>11.8501264027881</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>117.807128254595</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>0.23</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>1.955</v>
       </c>
-      <c r="W11" t="n">
+      <c r="X11" t="n">
         <v>8.3797</v>
       </c>
-      <c r="X11" t="n">
-        <v>0</v>
-      </c>
       <c r="Y11" t="n">
         <v>0</v>
       </c>
       <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
         <v>1.955</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AB11" t="n">
         <v>3.3626</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AC11" t="n">
         <v>1.20230337999802</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="n">
         <v>4.55</v>
       </c>
       <c r="C12" t="n">
+        <v>0.0000281838293126445</v>
+      </c>
+      <c r="D12" t="n">
         <v>8.8385</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>53.305</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>37.8565</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>342.446109500365</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>70.2353522688724</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>1089.55395976449</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>54.3716732254351</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>1.26456568560103</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>11.3735037762957</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>2.16130617353028</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>84.5027487726868</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>10.8964076184432</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>132.418593583131</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>1.62869231925625</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>44.7385493176498</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>0.619742860241292</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>14.2478883569473</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>69.3136955632509</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>0.2</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>1.7</v>
       </c>
-      <c r="W12" t="n">
+      <c r="X12" t="n">
         <v>8.51225</v>
       </c>
-      <c r="X12" t="n">
-        <v>0</v>
-      </c>
       <c r="Y12" t="n">
         <v>0</v>
       </c>
       <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
         <v>1.7</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AB12" t="n">
         <v>2.924</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AC12" t="n">
         <v>1.16089338376104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" t="n">
         <v>4.97</v>
       </c>
       <c r="C13" t="n">
+        <v>0.0000107151930523761</v>
+      </c>
+      <c r="D13" t="n">
         <v>8.43066666666667</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>39.3386666666667</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>52.2306666666667</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>207.063827314568</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>37.9451611857119</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>1226.78666398427</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>61.219954288351</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>0.338954984119721</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>3.04856112717277</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>5.82175813042596</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>227.619099383394</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>11.9831094778485</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>145.624737929554</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>1.67594257504849</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>46.0364665940071</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>0.192352087925877</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>4.42217450141591</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>79.556128968671</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>0.17</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>1.625</v>
       </c>
-      <c r="W13" t="n">
+      <c r="X13" t="n">
         <v>9.3319</v>
       </c>
-      <c r="X13" t="n">
-        <v>0</v>
-      </c>
       <c r="Y13" t="n">
         <v>0</v>
       </c>
       <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
         <v>1.625</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AB13" t="n">
         <v>2.795</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AC13" t="n">
         <v>1.31208436875774</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="n">
         <v>5.23</v>
       </c>
       <c r="C14" t="n">
+        <v>0.00000588843655355588</v>
+      </c>
+      <c r="D14" t="n">
         <v>7.517</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>38.1885</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>54.294</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>262.29745862695</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>60.1921245369108</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>1436.33433423746</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>71.6769466658743</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>0.0955872870933732</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.859712060117799</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>4.14195658752578</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>161.942218659083</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>14.0038971419735</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>170.182360017833</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>0.837867626852692</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>23.0153858420166</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>0.264765905270096</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>6.08696816215951</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>90.1831535877371</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>0.16</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>1.42</v>
       </c>
-      <c r="W14" t="n">
+      <c r="X14" t="n">
         <v>8.8523</v>
       </c>
-      <c r="X14" t="n">
-        <v>0</v>
-      </c>
       <c r="Y14" t="n">
         <v>0</v>
       </c>
       <c r="Z14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="n">
         <v>1.42</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AB14" t="n">
         <v>2.4424</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AC14" t="n">
         <v>1.34302407517501</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="n">
         <v>5.52</v>
       </c>
       <c r="C15" t="n">
+        <v>0.00000301995172040202</v>
+      </c>
+      <c r="D15" t="n">
         <v>11.9253333333333</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>67.6246666666667</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>20.4503333333333</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>300.046999810212</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>50.7777031679012</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>1987.90833958141</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>99.2019731314643</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>0.0966730647609436</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0.869477544459927</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>6.33996580005441</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>247.879982850527</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>18.230545417971</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>221.546703191892</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>0.356393119016962</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>9.78976258627694</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>0.689114536308426</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>15.8427431897307</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>124.558271950559</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>0.265</v>
       </c>
-      <c r="V15" t="n">
+      <c r="W15" t="n">
         <v>2.495</v>
       </c>
-      <c r="W15" t="n">
+      <c r="X15" t="n">
         <v>9.4264</v>
       </c>
-      <c r="X15" t="n">
-        <v>0</v>
-      </c>
       <c r="Y15" t="n">
         <v>0</v>
       </c>
       <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
         <v>2.495</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AB15" t="n">
         <v>4.2914</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AC15" t="n">
         <v>1.17879757935276</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" t="n">
         <v>5.37</v>
       </c>
       <c r="C16" t="n">
+        <v>0.00000426579518801593</v>
+      </c>
+      <c r="D16" t="n">
         <v>7.8455</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>52.9115</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>39.243</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>195.875766258963</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>48.4728510439506</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>1185.5305642888</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>59.1611639447478</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.0598329462721111</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.538137518771367</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>5.68767245474211</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>222.376617635507</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>8.32081241953481</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>101.118672928397</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>0.950271064335569</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>26.1029958662337</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>0.179181635415627</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>4.11938579820526</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>73.4086634007124</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>0.15</v>
       </c>
-      <c r="V16" t="n">
+      <c r="W16" t="n">
         <v>1.35</v>
       </c>
-      <c r="W16" t="n">
+      <c r="X16" t="n">
         <v>8.9766</v>
       </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
       <c r="Y16" t="n">
         <v>0</v>
       </c>
       <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
         <v>1.35</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AB16" t="n">
         <v>2.322</v>
       </c>
-      <c r="AB16" t="n">
+      <c r="AC16" t="n">
         <v>1.47751494790926</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" t="n">
         <v>5.58</v>
       </c>
       <c r="C17" t="n">
+        <v>0.00000263026799189538</v>
+      </c>
+      <c r="D17" t="n">
         <v>12.6705</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>54.38</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>32.9495</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>389.740445471421</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>86.3350326421948</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>1896.50029621024</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>94.6404659020029</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.048524185015795</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.436426520032061</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>9.65176469227504</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>377.364695938569</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>16.2650857815015</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>197.661454959697</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>0.966307877794072</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>26.5435110951254</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>0.91318595155872</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>20.994145026335</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>121.519026512354</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>0.25</v>
       </c>
-      <c r="V17" t="n">
+      <c r="W17" t="n">
         <v>2.27333333333333</v>
       </c>
-      <c r="W17" t="n">
+      <c r="X17" t="n">
         <v>9.06306666666667</v>
       </c>
-      <c r="X17" t="n">
-        <v>0</v>
-      </c>
       <c r="Y17" t="n">
         <v>0</v>
       </c>
       <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
         <v>2.27333333333333</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AB17" t="n">
         <v>3.91013333333333</v>
       </c>
-      <c r="AB17" t="n">
+      <c r="AC17" t="n">
         <v>1.19272306481298</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" t="n">
         <v>7.03</v>
       </c>
       <c r="C18" t="n">
+        <v>0.000000093325430079699</v>
+      </c>
+      <c r="D18" t="n">
         <v>18.0735</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>66.819</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>15.108</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>637.352431330765</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>123.596493197959</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>7205.47714331333</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>359.572690419349</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>-0.00372863698971526</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>-0.033535361085499</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>18.8311963527992</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>736.262115001743</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>19.916115751442</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>242.030596669399</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>0.164000276534334</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>4.50492359612162</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>0.79612679011392</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>18.302954904719</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>399.112400676714</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>0.51</v>
       </c>
-      <c r="V18" t="n">
+      <c r="W18" t="n">
         <v>5.425</v>
       </c>
-      <c r="W18" t="n">
+      <c r="X18" t="n">
         <v>10.57635</v>
       </c>
-      <c r="X18" t="n">
+      <c r="Y18" t="n">
         <v>0.39</v>
       </c>
-      <c r="Y18" t="n">
-        <v>0</v>
-      </c>
       <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
         <v>5.035</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AB18" t="n">
         <v>8.6602</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AC18" t="n">
         <v>1.0073465835549</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" t="n">
         <v>6.3</v>
       </c>
       <c r="C19" t="n">
+        <v>0.000000501187233627272</v>
+      </c>
+      <c r="D19" t="n">
         <v>9.451</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>52.5545</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>37.995</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>402.95296893361</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>83.965034453893</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>2443.00829806977</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>121.912685167412</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>-0.00334947233985975</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>-0.0301251542246986</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>9.63754018624557</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>376.808546201829</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>20.378892694265</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>247.654493467055</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>0.592063928887564</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>16.2634040626125</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>0.818122771154261</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>18.8086425088365</v>
       </c>
-      <c r="T19" t="n">
+      <c r="U19" t="n">
         <v>152.743891346737</v>
       </c>
-      <c r="U19" t="n">
+      <c r="V19" t="n">
         <v>0.27</v>
       </c>
-      <c r="V19" t="n">
+      <c r="W19" t="n">
         <v>2.5</v>
       </c>
-      <c r="W19" t="n">
+      <c r="X19" t="n">
         <v>9.25825</v>
       </c>
-      <c r="X19" t="n">
-        <v>0</v>
-      </c>
       <c r="Y19" t="n">
         <v>0</v>
       </c>
       <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
         <v>2.5</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AB19" t="n">
         <v>4.3</v>
       </c>
-      <c r="AB19" t="n">
+      <c r="AC19" t="n">
         <v>1.18204336919687</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" t="n">
         <v>5.43</v>
       </c>
       <c r="C20" t="n">
+        <v>0.00000371535229097173</v>
+      </c>
+      <c r="D20" t="n">
         <v>9.0425</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>61.5785</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>29.379</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>385.644256917096</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>77.7106491348642</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>1702.56701021484</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>84.9626732978112</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>0.104533683798466</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>0.940175952083404</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>7.41873778539208</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>290.05780993326</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>20.8602262466058</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>253.503899461877</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>0.731353521471481</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>20.0895498813001</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>0.307405118820565</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>7.06724368168479</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>113.653576132428</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>0.25</v>
       </c>
-      <c r="V20" t="n">
+      <c r="W20" t="n">
         <v>2.25333333333333</v>
       </c>
-      <c r="W20" t="n">
+      <c r="X20" t="n">
         <v>9.0446</v>
       </c>
-      <c r="X20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y20"/>
-      <c r="Z20" t="n">
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20"/>
+      <c r="AA20" t="n">
         <v>2.25333333333333</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AB20" t="n">
         <v>3.87573333333333</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AC20" t="n">
         <v>1.21858468066768</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" t="n">
         <v>4.44</v>
       </c>
       <c r="C21" t="n">
+        <v>0.0000363078054770101</v>
+      </c>
+      <c r="D21" t="n">
         <v>9.50533333333333</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>56.291</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>34.2036666666667</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>311.32644413203</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>66.8878972530041</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>1070.27250984542</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>53.4094770120974</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>2.02569156044518</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>18.219069894644</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>2.11367031050945</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>82.6402818002984</v>
       </c>
-      <c r="N21" t="n">
+      <c r="O21" t="n">
         <v>11.2861430581211</v>
       </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
         <v>137.154853513817</v>
       </c>
-      <c r="P21" t="n">
+      <c r="Q21" t="n">
         <v>1.10046384163951</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>30.2286412659957</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>0.817240765696225</v>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>18.7883652033562</v>
       </c>
-      <c r="T21" t="n">
+      <c r="U21" t="n">
         <v>69.6522227068694</v>
       </c>
-      <c r="U21" t="n">
+      <c r="V21" t="n">
         <v>0.195</v>
       </c>
-      <c r="V21" t="n">
+      <c r="W21" t="n">
         <v>1.64</v>
       </c>
-      <c r="W21" t="n">
+      <c r="X21" t="n">
         <v>8.3689</v>
       </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
       <c r="Y21" t="n">
         <v>0</v>
       </c>
       <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
         <v>1.64</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AB21" t="n">
         <v>2.8208</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AC21" t="n">
         <v>1.16561548446973</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="n">
         <v>6.73</v>
       </c>
       <c r="C22" t="n">
+        <v>0.000000186208713666287</v>
+      </c>
+      <c r="D22" t="n">
         <v>7.0325</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>39.714</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>53.253</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>347.513231391684</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>66.9540934089218</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>3118.15539167325</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>155.604341118481</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>-0.0019731369671345</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>-0.0177463938824077</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>9.63913660293301</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>376.870962901475</v>
       </c>
-      <c r="N22" t="n">
+      <c r="O22" t="n">
         <v>15.7121212405439</v>
       </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
         <v>190.941553375709</v>
       </c>
-      <c r="P22" t="n">
+      <c r="Q22" t="n">
         <v>0.410899433973458</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="R22" t="n">
         <v>11.2869965518169</v>
       </c>
-      <c r="R22" t="n">
+      <c r="S22" t="n">
         <v>0.338190050198549</v>
       </c>
-      <c r="S22" t="n">
+      <c r="T22" t="n">
         <v>7.77498925406464</v>
       </c>
-      <c r="T22" t="n">
+      <c r="U22" t="n">
         <v>181.29181587519</v>
       </c>
-      <c r="U22" t="n">
+      <c r="V22" t="n">
         <v>0.24</v>
       </c>
-      <c r="V22" t="n">
+      <c r="W22" t="n">
         <v>2.03</v>
       </c>
-      <c r="W22" t="n">
+      <c r="X22" t="n">
         <v>8.45935</v>
       </c>
-      <c r="X22" t="n">
-        <v>0</v>
-      </c>
       <c r="Y22" t="n">
         <v>0</v>
       </c>
       <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
         <v>2.03</v>
       </c>
-      <c r="AA22" t="n">
+      <c r="AB22" t="n">
         <v>3.4916</v>
       </c>
-      <c r="AB22" t="n">
+      <c r="AC22" t="n">
         <v>1.21581005386545</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" t="n">
         <v>5.16</v>
       </c>
       <c r="C23" t="n">
+        <v>0.00000691830970918936</v>
+      </c>
+      <c r="D23" t="n">
         <v>9.32166666666667</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>56.748</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>33.9306666666667</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>257.322594896198</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>47.9420024334486</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>1290.3352079037</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>64.3911975599432</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>0.202668473545949</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>1.82280025107226</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>3.32956171645026</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>130.179203989772</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>16.0788157066114</v>
       </c>
-      <c r="O23" t="n">
+      <c r="P23" t="n">
         <v>195.397807874595</v>
       </c>
-      <c r="P23" t="n">
+      <c r="Q23" t="n">
         <v>0.950913238041901</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="R23" t="n">
         <v>26.120635735773</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>0.32505375199891</v>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>7.47298575845495</v>
       </c>
-      <c r="T23" t="n">
+      <c r="U23" t="n">
         <v>84.3272972085497</v>
       </c>
-      <c r="U23" t="n">
+      <c r="V23" t="n">
         <v>0.205</v>
       </c>
-      <c r="V23" t="n">
+      <c r="W23" t="n">
         <v>1.77</v>
       </c>
-      <c r="W23" t="n">
+      <c r="X23" t="n">
         <v>8.8021</v>
       </c>
-      <c r="X23" t="n">
-        <v>0</v>
-      </c>
       <c r="Y23" t="n">
         <v>0</v>
       </c>
       <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
         <v>1.77</v>
       </c>
-      <c r="AA23" t="n">
+      <c r="AB23" t="n">
         <v>3.0444</v>
       </c>
-      <c r="AB23" t="n">
+      <c r="AC23" t="n">
         <v>1.24114815522917</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" t="n">
         <v>5.41</v>
       </c>
       <c r="C24" t="n">
+        <v>0.00000389045144994281</v>
+      </c>
+      <c r="D24" t="n">
         <v>9.503</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>52.612</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>37.8853333333333</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>384.658450703012</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>79.0398494654321</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>1833.08697564369</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>91.4759706394376</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>0.124319353977332</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>1.11812826967212</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>5.43502672001994</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>212.498674699339</v>
       </c>
-      <c r="N24" t="n">
+      <c r="O24" t="n">
         <v>12.2991275467923</v>
       </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
         <v>149.465147512393</v>
       </c>
-      <c r="P24" t="n">
+      <c r="Q24" t="n">
         <v>0.938742295984531</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="R24" t="n">
         <v>25.7863121283991</v>
       </c>
-      <c r="R24" t="n">
+      <c r="S24" t="n">
         <v>0.382992781996344</v>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>8.80500405809595</v>
       </c>
-      <c r="T24" t="n">
+      <c r="U24" t="n">
         <v>109.717437042223</v>
       </c>
-      <c r="U24" t="n">
+      <c r="V24" t="n">
         <v>0.22</v>
       </c>
-      <c r="V24" t="n">
+      <c r="W24" t="n">
         <v>1.94</v>
       </c>
-      <c r="W24" t="n">
+      <c r="X24" t="n">
         <v>8.7565</v>
       </c>
-      <c r="X24" t="n">
-        <v>0</v>
-      </c>
       <c r="Y24" t="n">
         <v>0</v>
       </c>
       <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
         <v>1.94</v>
       </c>
-      <c r="AA24" t="n">
+      <c r="AB24" t="n">
         <v>3.3368</v>
       </c>
-      <c r="AB24" t="n">
+      <c r="AC24" t="n">
         <v>1.2067009017223</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25" t="n">
         <v>7.18</v>
       </c>
       <c r="C25" t="n">
+        <v>0.0000000660693448007596</v>
+      </c>
+      <c r="D25" t="n">
         <v>13.351</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>66.8985</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>19.7515</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>782.762078727111</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>146.311570503045</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>8109.58902442154</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>404.690305126081</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>-0.00110732231119878</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>-0.00995925686692184</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>16.5838686322481</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>648.396095783635</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>17.2678491926067</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>209.847537313153</v>
       </c>
-      <c r="P25" t="n">
+      <c r="Q25" t="n">
         <v>0.161833796130833</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="R25" t="n">
         <v>4.44541254591785</v>
       </c>
-      <c r="R25" t="n">
+      <c r="S25" t="n">
         <v>0.632535579578378</v>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>14.5419929745069</v>
       </c>
-      <c r="T25" t="n">
+      <c r="U25" t="n">
         <v>439.173451208203</v>
       </c>
-      <c r="U25" t="n">
+      <c r="V25" t="n">
         <v>0.38</v>
       </c>
-      <c r="V25" t="n">
+      <c r="W25" t="n">
         <v>4.245</v>
       </c>
-      <c r="W25" t="n">
+      <c r="X25" t="n">
         <v>11.20645</v>
       </c>
-      <c r="X25" t="n">
+      <c r="Y25" t="n">
         <v>0.97</v>
       </c>
-      <c r="Y25" t="n">
-        <v>0</v>
-      </c>
       <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
         <v>3.275</v>
       </c>
-      <c r="AA25" t="n">
+      <c r="AB25" t="n">
         <v>5.633</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AC25" t="n">
         <v>1.08728724632844</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" t="n">
         <v>5.48</v>
       </c>
       <c r="C26" t="n">
+        <v>0.00000331131121482591</v>
+      </c>
+      <c r="D26" t="n">
         <v>9.18933333333333</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>44.6743333333333</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>46.1366666666667</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>240.931547101393</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>47.5670501690206</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>1806.05010849948</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>90.1267582463935</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>0.0327743620517251</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>0.294772612293216</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>4.30630789846404</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>168.368026214147</v>
       </c>
-      <c r="N26" t="n">
+      <c r="O26" t="n">
         <v>13.2884268838849</v>
       </c>
-      <c r="O26" t="n">
+      <c r="P26" t="n">
         <v>161.487607706411</v>
       </c>
-      <c r="P26" t="n">
+      <c r="Q26" t="n">
         <v>0.948187544890297</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="R26" t="n">
         <v>26.0457636705916</v>
       </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
         <v>0.274216242438621</v>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>6.30423141366389</v>
       </c>
-      <c r="T26" t="n">
+      <c r="U26" t="n">
         <v>108.028483633233</v>
       </c>
-      <c r="U26" t="n">
+      <c r="V26" t="n">
         <v>0.18</v>
       </c>
-      <c r="V26" t="n">
+      <c r="W26" t="n">
         <v>1.615</v>
       </c>
-      <c r="W26" t="n">
+      <c r="X26" t="n">
         <v>9.0096</v>
       </c>
-      <c r="X26" t="n">
-        <v>0</v>
-      </c>
       <c r="Y26" t="n">
         <v>0</v>
       </c>
       <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="n">
         <v>1.615</v>
       </c>
-      <c r="AA26" t="n">
+      <c r="AB26" t="n">
         <v>2.7778</v>
       </c>
-      <c r="AB26" t="n">
+      <c r="AC26" t="n">
         <v>1.29637893402817</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" t="n">
         <v>7.31</v>
       </c>
       <c r="C27" t="n">
+        <v>0.0000000489778819368447</v>
+      </c>
+      <c r="D27" t="n">
         <v>16.804</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>70.687</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>12.509</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>744.487706229807</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>127.406072509103</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>8049.64722726733</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>401.699048219339</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>-0.0178984964306015</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>-0.160979076896829</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>11.047488182486</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>431.934692958837</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>19.3442069998916</v>
       </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
         <v>235.080475566183</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>0.110380754161764</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>3.0320489360695</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>0.607867566770582</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>13.9748753600557</v>
       </c>
-      <c r="T27" t="n">
+      <c r="U27" t="n">
         <v>432.680712472056</v>
       </c>
-      <c r="U27" t="n">
+      <c r="V27" t="n">
         <v>0.28</v>
       </c>
-      <c r="V27" t="n">
+      <c r="W27" t="n">
         <v>4.65</v>
       </c>
-      <c r="W27" t="n">
+      <c r="X27" t="n">
         <v>16.6295</v>
       </c>
-      <c r="X27" t="n">
+      <c r="Y27" t="n">
         <v>2.33</v>
       </c>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
       <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
         <v>2.32</v>
       </c>
-      <c r="AA27" t="n">
+      <c r="AB27" t="n">
         <v>3.9904</v>
       </c>
-      <c r="AB27" t="n">
+      <c r="AC27" t="n">
         <v>1.17026429314969</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="n">
         <v>6.81</v>
       </c>
       <c r="C28" t="n">
+        <v>0.000000154881661891248</v>
+      </c>
+      <c r="D28" t="n">
         <v>18.4803333333333</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>67.994</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>13.5256666666667</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>379.428265481482</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>86.877073657679</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>5511.50367149464</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>275.038857802018</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>-0.00691095029674439</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>-0.0621570869689191</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>6.54553528811404</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>255.917338694683</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>29.9131111280033</v>
       </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
         <v>363.51908298306</v>
       </c>
-      <c r="P28" t="n">
+      <c r="Q28" t="n">
         <v>0.281896429141579</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="R28" t="n">
         <v>7.74341301209002</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>0.685472307243824</v>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>15.7590083435355</v>
       </c>
-      <c r="T28" t="n">
+      <c r="U28" t="n">
         <v>312.176065575083</v>
       </c>
-      <c r="U28" t="n">
+      <c r="V28" t="n">
         <v>0.375</v>
       </c>
-      <c r="V28" t="n">
+      <c r="W28" t="n">
         <v>3.46</v>
       </c>
-      <c r="W28" t="n">
+      <c r="X28" t="n">
         <v>9.2322</v>
       </c>
-      <c r="X28" t="n">
-        <v>0</v>
-      </c>
       <c r="Y28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="n">
         <v>71.93275</v>
       </c>
-      <c r="Z28" t="n">
+      <c r="AA28" t="n">
         <v>3.46</v>
       </c>
-      <c r="AA28" t="n">
+      <c r="AB28" t="n">
         <v>5.9512</v>
       </c>
-      <c r="AB28" t="n">
+      <c r="AC28" t="n">
         <v>1.10592436220753</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" t="n">
         <v>4.6</v>
       </c>
       <c r="C29" t="n">
+        <v>0.0000251188643150958</v>
+      </c>
+      <c r="D29" t="n">
         <v>8.7045</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>52.765</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>38.5305</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>155.349010146291</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>20.2374777032428</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>1046.10716595802</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>52.203561353262</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>1.41943348723472</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>12.7663847841891</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>2.4619695442523</v>
       </c>
-      <c r="M29" t="n">
+      <c r="N29" t="n">
         <v>96.2580852411764</v>
       </c>
-      <c r="N29" t="n">
+      <c r="O29" t="n">
         <v>10.6630801847792</v>
       </c>
-      <c r="O29" t="n">
+      <c r="P29" t="n">
         <v>129.58308194553</v>
       </c>
-      <c r="P29" t="n">
+      <c r="Q29" t="n">
         <v>1.64700671272871</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="R29" t="n">
         <v>45.2416273919448</v>
       </c>
-      <c r="R29" t="n">
+      <c r="S29" t="n">
         <v>0.778629008247692</v>
       </c>
-      <c r="S29" t="n">
+      <c r="T29" t="n">
         <v>17.9006808996144</v>
       </c>
-      <c r="T29" t="n">
+      <c r="U29" t="n">
         <v>67.5266735777759</v>
       </c>
-      <c r="U29" t="n">
+      <c r="V29" t="n">
         <v>0.2</v>
       </c>
-      <c r="V29" t="n">
+      <c r="W29" t="n">
         <v>1.66</v>
       </c>
-      <c r="W29" t="n">
+      <c r="X29" t="n">
         <v>8.4875</v>
       </c>
-      <c r="X29" t="n">
-        <v>0</v>
-      </c>
       <c r="Y29" t="n">
         <v>0</v>
       </c>
       <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
         <v>1.66</v>
       </c>
-      <c r="AA29" t="n">
+      <c r="AB29" t="n">
         <v>2.8552</v>
       </c>
-      <c r="AB29" t="n">
+      <c r="AC29" t="n">
         <v>1.21475255459366</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" t="n">
         <v>5.26</v>
       </c>
       <c r="C30" t="n">
+        <v>0.00000549540873857625</v>
+      </c>
+      <c r="D30" t="n">
         <v>8.153</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>58.907</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>32.9405</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>424.747315903526</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>92.8965074337448</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>1822.86943171827</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>90.9660877148693</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>0.0504638539812077</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>0.453871902706982</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>6.64490917530223</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>259.802658935967</v>
       </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
         <v>16.0425336120293</v>
       </c>
-      <c r="O30" t="n">
+      <c r="P30" t="n">
         <v>194.956889720186</v>
       </c>
-      <c r="P30" t="n">
+      <c r="Q30" t="n">
         <v>0.126122128934108</v>
       </c>
-      <c r="Q30" t="n">
+      <c r="R30" t="n">
         <v>3.464448759691</v>
       </c>
-      <c r="R30" t="n">
+      <c r="S30" t="n">
         <v>0.466340419716625</v>
       </c>
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>10.7211662492852</v>
       </c>
-      <c r="T30" t="n">
+      <c r="U30" t="n">
         <v>114.170334775899</v>
       </c>
-      <c r="U30" t="n">
+      <c r="V30" t="n">
         <v>0.19</v>
       </c>
-      <c r="V30" t="n">
+      <c r="W30" t="n">
         <v>1.69</v>
       </c>
-      <c r="W30" t="n">
+      <c r="X30" t="n">
         <v>8.97026666666667</v>
       </c>
-      <c r="X30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y30"/>
-      <c r="Z30" t="n">
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30"/>
+      <c r="AA30" t="n">
         <v>1.69</v>
       </c>
-      <c r="AA30" t="n">
+      <c r="AB30" t="n">
         <v>2.9068</v>
       </c>
-      <c r="AB30" t="n">
+      <c r="AC30" t="n">
         <v>1.35731602077892</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" t="n">
         <v>7</v>
       </c>
       <c r="C31" t="n">
+        <v>0.0000001</v>
+      </c>
+      <c r="D31" t="n">
         <v>14.811</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>64.0795</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>21.109</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>700.936894831961</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>142.048297021498</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>7658.30636356034</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>382.170086509324</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>0.0157789488645717</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>0.141915866087958</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>14.071237014934</v>
       </c>
-      <c r="M31" t="n">
+      <c r="N31" t="n">
         <v>550.157224809889</v>
       </c>
-      <c r="N31" t="n">
+      <c r="O31" t="n">
         <v>18.0264347957148</v>
       </c>
-      <c r="O31" t="n">
+      <c r="P31" t="n">
         <v>219.066248854924</v>
       </c>
-      <c r="P31" t="n">
+      <c r="Q31" t="n">
         <v>0.187787358611276</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="R31" t="n">
         <v>5.15833095369315</v>
       </c>
-      <c r="R31" t="n">
+      <c r="S31" t="n">
         <v>0.80945501174817</v>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>18.6093707200904</v>
       </c>
-      <c r="T31" t="n">
+      <c r="U31" t="n">
         <v>415.092992280585</v>
       </c>
-      <c r="U31" t="n">
+      <c r="V31" t="n">
         <v>0.405</v>
       </c>
-      <c r="V31" t="n">
+      <c r="W31" t="n">
         <v>3.76</v>
       </c>
-      <c r="W31" t="n">
+      <c r="X31" t="n">
         <v>9.3597</v>
       </c>
-      <c r="X31" t="n">
-        <v>0</v>
-      </c>
       <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
         <v>396.8372</v>
       </c>
-      <c r="Z31" t="n">
+      <c r="AA31" t="n">
         <v>3.76</v>
       </c>
-      <c r="AA31" t="n">
+      <c r="AB31" t="n">
         <v>6.4672</v>
       </c>
-      <c r="AB31" t="n">
+      <c r="AC31" t="n">
         <v>1.06022154714447</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" t="n">
         <v>6.97</v>
       </c>
       <c r="C32" t="n">
+        <v>0.000000107151930523761</v>
+      </c>
+      <c r="D32" t="n">
         <v>16.4123333333333</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>68.5543333333333</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>15.0333333333333</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>530.715935987516</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>104.558396548214</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>5988.52839885276</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>298.843674776823</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>-0.0135417630547703</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>-0.121794616914604</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>15.26453373822</v>
       </c>
-      <c r="M32" t="n">
+      <c r="N32" t="n">
         <v>596.812740096926</v>
       </c>
-      <c r="N32" t="n">
+      <c r="O32" t="n">
         <v>17.5466792154958</v>
       </c>
-      <c r="O32" t="n">
+      <c r="P32" t="n">
         <v>213.236019166312</v>
       </c>
-      <c r="P32" t="n">
+      <c r="Q32" t="n">
         <v>0.23468183342423</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="R32" t="n">
         <v>6.44647528233018</v>
       </c>
-      <c r="R32" t="n">
+      <c r="S32" t="n">
         <v>0.627534835399836</v>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>14.4270258658422</v>
       </c>
-      <c r="T32" t="n">
+      <c r="U32" t="n">
         <v>332.268880802884</v>
       </c>
-      <c r="U32" t="n">
+      <c r="V32" t="n">
         <v>0.425</v>
       </c>
-      <c r="V32" t="n">
+      <c r="W32" t="n">
         <v>4.27</v>
       </c>
-      <c r="W32" t="n">
+      <c r="X32" t="n">
         <v>10.0424</v>
       </c>
-      <c r="X32" t="n">
-        <v>0</v>
-      </c>
       <c r="Y32" t="n">
         <v>0</v>
       </c>
       <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
         <v>4.27</v>
       </c>
-      <c r="AA32" t="n">
+      <c r="AB32" t="n">
         <v>7.3444</v>
       </c>
-      <c r="AB32" t="n">
+      <c r="AC32" t="n">
         <v>1.02786835160155</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" t="n">
         <v>5.18</v>
       </c>
       <c r="C33" t="n">
+        <v>0.00000660693448007596</v>
+      </c>
+      <c r="D33" t="n">
         <v>10.4626666666667</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>47.628</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>41.9096666666667</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>458.796692730232</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>105.241381566683</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>2069.17867708706</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>103.257581570291</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>0.188988448904703</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>1.6997621094489</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>2.85094293036116</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>111.46616669126</v>
       </c>
-      <c r="N33" t="n">
+      <c r="O33" t="n">
         <v>10.6335706618196</v>
       </c>
-      <c r="O33" t="n">
+      <c r="P33" t="n">
         <v>129.224467467763</v>
       </c>
-      <c r="P33" t="n">
+      <c r="Q33" t="n">
         <v>0.526852874819069</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="R33" t="n">
         <v>14.472121618405</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S33" t="n">
         <v>0.365907210908788</v>
       </c>
-      <c r="S33" t="n">
+      <c r="T33" t="n">
         <v>8.41220677879304</v>
       </c>
-      <c r="T33" t="n">
+      <c r="U33" t="n">
         <v>117.296990822285</v>
       </c>
-      <c r="U33" t="n">
+      <c r="V33" t="n">
         <v>0.28</v>
       </c>
-      <c r="V33" t="n">
+      <c r="W33" t="n">
         <v>2.65</v>
       </c>
-      <c r="W33" t="n">
+      <c r="X33" t="n">
         <v>9.5904</v>
       </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
       <c r="Y33" t="n">
         <v>0</v>
       </c>
       <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
         <v>2.65</v>
       </c>
-      <c r="AA33" t="n">
+      <c r="AB33" t="n">
         <v>4.558</v>
       </c>
-      <c r="AB33" t="n">
+      <c r="AC33" t="n">
         <v>1.24093874943277</v>
       </c>
     </row>

</xml_diff>